<commit_message>
hazırlana excel dosyasının uzantısı ekrana yazdırıp inderme linki oluşturma ve JUnive başlangıcı
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DormitoryProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD68E7D-03D4-41B1-BC01-43949E4A809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D678513-0916-4688-A8E4-D0E96EC86CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="54">
   <si>
     <t>Succes</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>İd değerine göre öğrenci bulunamadı</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
 </sst>
 </file>
@@ -209,8 +218,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,30 +557,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="15.33203125"/>
-    <col min="3" max="3" customWidth="true" width="35.44140625"/>
+    <col min="3" max="3" customWidth="true" width="59.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="0">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>0</v>
@@ -579,7 +593,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>0</v>
@@ -590,7 +604,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>0</v>
@@ -601,29 +615,29 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>0</v>
@@ -634,73 +648,73 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s" s="0">
         <v>0</v>
@@ -711,106 +725,106 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>0</v>
@@ -821,7 +835,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s" s="0">
         <v>0</v>
@@ -832,7 +846,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s" s="0">
         <v>0</v>
@@ -843,7 +857,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s" s="0">
         <v>0</v>
@@ -854,7 +868,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s" s="0">
         <v>0</v>
@@ -865,7 +879,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s" s="0">
         <v>0</v>
@@ -876,7 +890,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>0</v>
@@ -887,7 +901,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s" s="0">
         <v>0</v>
@@ -898,7 +912,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s" s="0">
         <v>0</v>
@@ -909,18 +923,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s" s="0">
         <v>0</v>
@@ -931,51 +945,51 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s" s="0">
         <v>0</v>
@@ -986,7 +1000,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="0">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s" s="0">
         <v>0</v>
@@ -997,29 +1011,29 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s" s="0">
         <v>0</v>
@@ -1030,7 +1044,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s" s="0">
         <v>0</v>
@@ -1041,7 +1055,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s" s="0">
         <v>0</v>
@@ -1052,7 +1066,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s" s="0">
         <v>0</v>
@@ -1063,7 +1077,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="0">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s" s="0">
         <v>0</v>
@@ -1074,40 +1088,40 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="0">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="0">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s" s="0">
         <v>0</v>
@@ -1118,7 +1132,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="0">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s" s="0">
         <v>0</v>
@@ -1129,7 +1143,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="0">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s" s="0">
         <v>0</v>
@@ -1140,7 +1154,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s" s="0">
         <v>0</v>
@@ -1151,51 +1165,51 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="0">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s" s="0">
         <v>0</v>
@@ -1206,29 +1220,29 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="0">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="0">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="0">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s" s="0">
         <v>0</v>
@@ -1239,7 +1253,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="0">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s" s="0">
         <v>0</v>
@@ -1250,40 +1264,40 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="0">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="0">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="0">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s" s="0">
         <v>0</v>
@@ -1294,84 +1308,84 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="0">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="0">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="0">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="0">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="0">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="0">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="0">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="0">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s" s="0">
         <v>4</v>
@@ -1382,18 +1396,18 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="0">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="0">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s" s="0">
         <v>4</v>
@@ -1404,7 +1418,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="0">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s" s="0">
         <v>4</v>
@@ -1415,73 +1429,73 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="0">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="0">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="0">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="0">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="0">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s" s="0">
         <v>0</v>
@@ -1492,7 +1506,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="0">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s" s="0">
         <v>0</v>
@@ -1503,7 +1517,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="0">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s" s="0">
         <v>0</v>
@@ -1514,7 +1528,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="0">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s" s="0">
         <v>0</v>
@@ -1525,7 +1539,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="0">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s" s="0">
         <v>0</v>
@@ -1536,7 +1550,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="0">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s" s="0">
         <v>0</v>
@@ -1547,7 +1561,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="0">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s" s="0">
         <v>0</v>
@@ -1558,73 +1572,73 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="0">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="0">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="0">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="0">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="0">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="0">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s" s="0">
         <v>4</v>
@@ -1635,7 +1649,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="0">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s" s="0">
         <v>4</v>
@@ -1646,106 +1660,106 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="0">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="0">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="0">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="0">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="0">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="0">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="0">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="0">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C107" t="s" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="0">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="0">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s" s="0">
         <v>14</v>
@@ -1756,51 +1770,51 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="0">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="0">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="0">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="0">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="0">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s" s="0">
         <v>0</v>
@@ -1811,7 +1825,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="0">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s" s="0">
         <v>0</v>
@@ -1822,51 +1836,51 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="0">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="0">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C117" t="s" s="0">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="0">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C118" t="s" s="0">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="0">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="0">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s" s="0">
         <v>0</v>
@@ -1877,7 +1891,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="0">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s" s="0">
         <v>0</v>
@@ -1888,7 +1902,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="0">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s" s="0">
         <v>0</v>
@@ -1899,7 +1913,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="0">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s" s="0">
         <v>0</v>
@@ -1910,7 +1924,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="0">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s" s="0">
         <v>0</v>
@@ -1921,7 +1935,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="0">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s" s="0">
         <v>0</v>
@@ -1932,51 +1946,51 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="0">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="0">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="0">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128" t="s" s="0">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="0">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B129" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="0">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B130" t="s" s="0">
         <v>4</v>
@@ -1987,7 +2001,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="0">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s" s="0">
         <v>4</v>
@@ -1998,29 +2012,29 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="0">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="0">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s" s="0">
         <v>0</v>
       </c>
       <c r="C133" t="s" s="0">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="0">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134" t="s" s="0">
         <v>0</v>
@@ -2031,18 +2045,18 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="0">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C135" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="0">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s" s="0">
         <v>4</v>
@@ -2053,106 +2067,106 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="0">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="0">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="0">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="0">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="0">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C141" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="0">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="0">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C143" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="0">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s" s="0">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C144" t="s" s="0">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="0">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B145" t="s" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C145" t="s" s="0">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="0">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B146" t="s" s="0">
         <v>4</v>
@@ -2161,47 +2175,58 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" t="n" s="0">
-        <v>147.0</v>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="0">
+        <v>146</v>
       </c>
       <c r="B147" t="s" s="0">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C147" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n" s="0">
-        <v>148.0</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="0">
+        <v>147</v>
       </c>
       <c r="B148" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C148" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n" s="0">
-        <v>149.0</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="0">
+        <v>148</v>
       </c>
       <c r="B149" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C149" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="0">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C150" t="s" s="0">
         <v>36</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" t="n" s="0">
-        <v>150.0</v>
-      </c>
-      <c r="B150" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C150" t="s" s="0">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="0">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s" s="0">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
epoch timestamp türünde gelen tarih verisini normal Date formatına çevirmek
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DormitoryProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9FE271-3293-4DF7-B16E-CD5501B451CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DB0E61-5E4C-45A2-876F-D000B705072B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -47,13 +47,30 @@
   </si>
   <si>
     <t>Tüm öğrenciler listelendi</t>
+  </si>
+  <si>
+    <t>Tüm personeller listelendi</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Girilen id değerine ait bir personel bulunamadı</t>
+  </si>
+  <si>
+    <t>İd değerine göre personel listelendi</t>
+  </si>
+  <si>
+    <t>Kiralamalar listelendi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd-MM-yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,11 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,17 +440,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.44140625"/>
     <col min="2" max="2" customWidth="true" width="21.6640625"/>
-    <col min="3" max="3" customWidth="true" width="33.21875"/>
+    <col min="3" max="3" customWidth="true" width="45.44140625"/>
     <col min="4" max="4" customWidth="true" width="19.0"/>
   </cols>
   <sheetData>
@@ -450,9 +468,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>159.0</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
+        <v>159</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>4</v>
@@ -460,13 +478,13 @@
       <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>160.0</v>
+      <c r="D2" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
+        <v>160</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>6</v>
@@ -474,13 +492,13 @@
       <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D3" t="n" s="0">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>161.0</v>
+      <c r="D3" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
+        <v>161</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>6</v>
@@ -488,7 +506,133 @@
       <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D4" t="n" s="0">
+      <c r="D4" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="0">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="0">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="0">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="0">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D8" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="0">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="0">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="0">
+        <v>168</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D11" s="0">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>169.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n" s="2">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>170.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n" s="2">
         <v>45575.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mail gönderme işlemi(değiştirilecek ve geliştirilecek
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>Id</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Kiralamalar listelendi</t>
+  </si>
+  <si>
+    <t>İd değerine göre departman listeleme işlemi başarılı</t>
+  </si>
+  <si>
+    <t>Departman ekleme işlemi başarılı</t>
+  </si>
+  <si>
+    <t>Bu id değerine ait bir departman bulunamadı.</t>
   </si>
 </sst>
 </file>
@@ -100,11 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -440,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -636,6 +647,118 @@
         <v>45575.0</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>171.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D14" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="0">
+        <v>172.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D15" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="0">
+        <v>173.0</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="0">
+        <v>174.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>175.0</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>176.0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D19" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>177.0</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D20" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>178.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D21" t="n" s="3">
+        <v>45575.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dao hazır sorgu çalışması : baş harf değerine göre departman listeleme
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DormitoryProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DB0E61-5E4C-45A2-876F-D000B705072B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5816EB2-3BF4-43DD-9237-DA78890362B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>Bu id değerine ait bir departman bulunamadı.</t>
+  </si>
+  <si>
+    <t>İd değerine göre öğrenci listelendi</t>
+  </si>
+  <si>
+    <t>İd değerine göre öğrenci bulunamadı</t>
+  </si>
+  <si>
+    <t>Aynı getMaildeğerine sahip öğrenci bulunda</t>
+  </si>
+  <si>
+    <t>Mail veya kimlik nummarası benzersiz olmalıdır</t>
+  </si>
+  <si>
+    <t>Öğrenci güncelleme işlemi başarılı</t>
+  </si>
+  <si>
+    <t>Öğrenci ekleme işlemi başarılı</t>
+  </si>
+  <si>
+    <t>Baş harfi değerine göre departman veya departmanlar başarılı şekilde listelendi</t>
+  </si>
+  <si>
+    <t>Bu harf ile başlayan departman departman bulunamadı</t>
   </si>
 </sst>
 </file>
@@ -78,7 +102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd-MM-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,14 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,312 +473,1334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.44140625"/>
-    <col min="2" max="2" customWidth="true" width="21.6640625"/>
-    <col min="3" max="3" customWidth="true" width="45.44140625"/>
-    <col min="4" max="4" customWidth="true" width="19.0"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>159</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>45575</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>160</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>45575</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>161</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>45575</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>162</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>45575</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>163</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>45575</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>164</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>45575</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>165</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>45575</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>166</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>45575</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>167</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>45575</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>168</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0">
-        <v>45575</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n" s="0">
-        <v>169.0</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s" s="0">
+      <c r="D11">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>169</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="n" s="2">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n" s="0">
-        <v>170.0</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s" s="0">
+      <c r="D12" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>170</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="n" s="2">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n" s="0">
-        <v>171.0</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s" s="0">
+      <c r="D13" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>171</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n" s="0">
-        <v>172.0</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s" s="0">
+      <c r="D14" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>172</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n" s="0">
-        <v>173.0</v>
-      </c>
-      <c r="B16" t="s" s="0">
+      <c r="D15" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>173</v>
+      </c>
+      <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n" s="0">
-        <v>174.0</v>
-      </c>
-      <c r="B17" t="s" s="0">
+      <c r="D16" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>174</v>
+      </c>
+      <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n" s="0">
-        <v>175.0</v>
-      </c>
-      <c r="B18" t="s" s="0">
+      <c r="D17" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="D18" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n" s="0">
-        <v>176.0</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s" s="0">
+      <c r="D18" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>176</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n" s="0">
-        <v>177.0</v>
-      </c>
-      <c r="B20" t="s" s="0">
+      <c r="D19" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>177</v>
+      </c>
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" t="n" s="3">
-        <v>45575.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n" s="0">
-        <v>178.0</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s" s="0">
+      <c r="D20" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" t="n" s="3">
-        <v>45575.0</v>
+      <c r="D21" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>179</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>180</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>181</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>182</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="2">
+        <v>45577</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>183</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>184</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>185</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>186</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>187</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>188</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>189</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>190</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>191</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>192</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>193</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>194</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>195</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>196</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>197</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>198</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>199</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>200</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>201</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>203</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>204</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>205</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>206</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="2">
+        <v>45581</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>207</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>208</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>209</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>210</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>211</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>212</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>213</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>214</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>215</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>216</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>217</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>218</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>219</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>220</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>221</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>222</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>223</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>224</v>
+      </c>
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>225</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>226</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>227</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>228</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>229</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>230</v>
+      </c>
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>231</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>232</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>233</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>234</v>
+      </c>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>235</v>
+      </c>
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D78" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>236</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>238</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>239</v>
+      </c>
+      <c r="B82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>240</v>
+      </c>
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>241</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>242</v>
+      </c>
+      <c r="B85" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>243</v>
+      </c>
+      <c r="B86" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>244</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="2">
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>245</v>
+      </c>
+      <c r="B88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>246</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>247</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>248</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D91" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>249</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>23</v>
+      </c>
+      <c r="D92" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>250</v>
+      </c>
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="2">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>251</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94" s="2">
+        <v>45583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>